<commit_message>
need to except 4
</commit_message>
<xml_diff>
--- a/actions.xlsx
+++ b/actions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33651\Desktop\Open Classrooms\P7_BELLEGUEULE_Pierre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0810C8-BAD4-4281-9807-485EBD72DF61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57BCFC47-FE88-46E8-B3C4-88F514B8B015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="3770" windowWidth="28800" windowHeight="15460" xr2:uid="{3398FCD7-BB1F-4776-9F03-45EE751A7F14}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3398FCD7-BB1F-4776-9F03-45EE751A7F14}"/>
   </bookViews>
   <sheets>
     <sheet name="actions" sheetId="1" r:id="rId1"/>
@@ -466,15 +466,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84541A0-6B9D-4DCF-9CA9-FDF0942C8DC0}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:C21"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,84 +485,112 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f>B2*C2/100</f>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>18</v>
+      </c>
+      <c r="C3">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="D3">
+        <f t="shared" ref="D3:D21" si="0">B3*C3/100</f>
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
         <v>20</v>
       </c>
-      <c r="C2">
+      <c r="C4">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>110</v>
+      </c>
+      <c r="C7">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="B8">
         <v>30</v>
       </c>
-      <c r="C3">
+      <c r="C8">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>50</v>
-      </c>
-      <c r="C4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>70</v>
-      </c>
-      <c r="C5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>60</v>
-      </c>
-      <c r="C6">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>80</v>
-      </c>
-      <c r="C7">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>22</v>
-      </c>
-      <c r="C8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -572,155 +600,210 @@
       <c r="C9">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>48</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>6.24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>14</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>60</v>
+      </c>
+      <c r="C14">
+        <v>17</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>42</v>
+      </c>
+      <c r="C15">
+        <v>17</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>7.14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16">
+        <v>114</v>
+      </c>
+      <c r="C16">
+        <v>18</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>20.52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>70</v>
+      </c>
+      <c r="C17">
+        <v>20</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>24</v>
+      </c>
+      <c r="C18">
+        <v>21</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>5.04</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>38</v>
+      </c>
+      <c r="C19">
+        <v>23</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>8.74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>80</v>
+      </c>
+      <c r="C20">
+        <v>25</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
+      <c r="B21">
         <v>34</v>
       </c>
-      <c r="C11">
+      <c r="C21">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12">
-        <v>42</v>
-      </c>
-      <c r="C12">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13">
-        <v>110</v>
-      </c>
-      <c r="C13">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14">
-        <v>38</v>
-      </c>
-      <c r="C14">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15">
-        <v>14</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16">
-        <v>18</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17">
-        <v>8</v>
-      </c>
-      <c r="C17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18">
-        <v>4</v>
-      </c>
-      <c r="C18">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19">
-        <v>10</v>
-      </c>
-      <c r="C19">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20">
-        <v>24</v>
-      </c>
-      <c r="C20">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21">
-        <v>114</v>
-      </c>
-      <c r="C21">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>9.18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C21">
+    <sortCondition ref="C2:C21"/>
+  </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>